<commit_message>
updated framework folder structure
</commit_message>
<xml_diff>
--- a/test-data/TestData.xlsx
+++ b/test-data/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BitBucket_Repositories\SanitySuite\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44E7F63-65D3-411F-B1F1-461996A755AC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA00093-750F-4833-AC94-9B68A2355490}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1509,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AJ6" sqref="AJ6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated Automation tickets assined 44,49,50,51
</commit_message>
<xml_diff>
--- a/test-data/TestData.xlsx
+++ b/test-data/TestData.xlsx
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3245" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3253" uniqueCount="358">
   <si>
     <t>test_name</t>
   </si>
@@ -1139,6 +1139,18 @@
   </si>
   <si>
     <t>AccountSearch</t>
+  </si>
+  <si>
+    <t>Associate_Account_To_Reservation</t>
+  </si>
+  <si>
+    <t>Ageing_Pay_Individual_Items_CashOrCard</t>
+  </si>
+  <si>
+    <t>Ageing_AutoApply</t>
+  </si>
+  <si>
+    <t>Ageing_AdvanceDeposit</t>
   </si>
 </sst>
 </file>
@@ -1582,15 +1594,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="A28" sqref="A28:A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1862,6 +1874,38 @@
         <v>353</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="31" t="s">
+        <v>354</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="31" t="s">
+        <v>356</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="31" t="s">
+        <v>357</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1900,6 +1944,10 @@
     <hyperlink ref="A32" r:id="rId31" location="RateQuote_Book_Reservation!A1"/>
     <hyperlink ref="A33" r:id="rId32" location="'Account Cash Payment'!A1"/>
     <hyperlink ref="A34" r:id="rId33" location="AccountSearch!A1"/>
+    <hyperlink ref="A35" r:id="rId34" location="AssociateAccountToReservation!A1"/>
+    <hyperlink ref="A36" r:id="rId35" location="Ageing_ItemLeavel!A1"/>
+    <hyperlink ref="A37" r:id="rId36" location="Ageing_AutoApply!A1"/>
+    <hyperlink ref="A38" r:id="rId37" location="Ageing_AdvanceDeposit!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12555,7 +12603,7 @@
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13318,7 +13366,7 @@
   <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated from develop branch
</commit_message>
<xml_diff>
--- a/test-data/TestData.xlsx
+++ b/test-data/TestData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BitBucket_Repositories\InnCenterRegression\inncenter.nextgen.automation\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rep\inncenter.nextgen.automation\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B8F88B-C7FF-4C67-948F-85E9006F699B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" firstSheet="42" activeTab="43"/>
   </bookViews>
   <sheets>
     <sheet name="testcases" sheetId="1" r:id="rId1"/>
@@ -67,6 +66,7 @@
     <sheet name="Ageing_AdvanceDeposit" sheetId="75" r:id="rId52"/>
     <sheet name="Ageing_AutoApply" sheetId="76" r:id="rId53"/>
     <sheet name="Ageing_ItemLeavel" sheetId="77" r:id="rId54"/>
+    <sheet name="Move Folio Accross Reservations" sheetId="78" r:id="rId55"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3241" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3393" uniqueCount="362">
   <si>
     <t>test_name</t>
   </si>
@@ -1082,27 +1082,12 @@
     <t>AmountToPay</t>
   </si>
   <si>
-    <t>House Accountt</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>resNumber1</t>
-  </si>
-  <si>
-    <t>10800334</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Address2</t>
   </si>
   <si>
     <t>Group</t>
   </si>
   <si>
-    <t>TestAccount</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
@@ -1134,12 +1119,57 @@
   </si>
   <si>
     <t>RateQuote_Book_Reservation</t>
+  </si>
+  <si>
+    <t>Accounts_Payment_Cash</t>
+  </si>
+  <si>
+    <t>AccountSearch</t>
+  </si>
+  <si>
+    <t>Associate_Account_To_Reservation</t>
+  </si>
+  <si>
+    <t>Ageing_Pay_Individual_Items_CashOrCard</t>
+  </si>
+  <si>
+    <t>Ageing_AutoApply</t>
+  </si>
+  <si>
+    <t>Ageing_AdvanceDeposit</t>
+  </si>
+  <si>
+    <t>MoveFolioItems</t>
+  </si>
+  <si>
+    <t>https://training.innroad.com/login.html</t>
+  </si>
+  <si>
+    <t>MoveFolioItemsAccrossReservations</t>
+  </si>
+  <si>
+    <t>Test Corp Acc</t>
+  </si>
+  <si>
+    <t>Test  Acc</t>
+  </si>
+  <si>
+    <t>Test Acc</t>
+  </si>
+  <si>
+    <t>guest</t>
+  </si>
+  <si>
+    <t>TestCorpAcc</t>
+  </si>
+  <si>
+    <t>auto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1225,7 +1255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1261,6 +1291,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1575,16 +1607,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1805,7 +1837,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>5</v>
@@ -1813,7 +1845,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>5</v>
@@ -1821,7 +1853,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>5</v>
@@ -1829,7 +1861,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>5</v>
@@ -1837,52 +1869,124 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="31" t="s">
+        <v>347</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="31" t="s">
+        <v>348</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="31" t="s">
+        <v>349</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="31" t="s">
+        <v>350</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="31" t="s">
         <v>351</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B37" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="31" t="s">
+        <v>352</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="31" t="s">
+        <v>353</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" location="Clean_Room_Classes!A1" xr:uid="{A3A5EEF2-DED3-4FD7-9A98-737659F390BE}"/>
-    <hyperlink ref="A3" r:id="rId2" location="Delete_Reservation!A1" xr:uid="{F62C86D1-86E9-43D0-94C0-CBCEE289D4DC}"/>
-    <hyperlink ref="A4" r:id="rId3" location="Create_New_Policy!A1" xr:uid="{2BF02B07-3931-4CE0-893F-9A685136A741}"/>
-    <hyperlink ref="A5" r:id="rId4" location="RetainPaymentInfoAfterEdit!A1" xr:uid="{48994CEF-E520-4ED2-8978-D670FE592AAA}"/>
-    <hyperlink ref="A6" r:id="rId5" location="VerifyItemDetail!A1" xr:uid="{6489588E-1A00-4751-A21E-EE1B42909EAC}"/>
-    <hyperlink ref="A7" r:id="rId6" location="VerifySaveBtnFuncForReservation!A1" xr:uid="{4C52BE03-273D-4BA5-8D49-ECF1A6710AC8}"/>
-    <hyperlink ref="A8" r:id="rId7" location="VerifySaveBtnFuncForAccounts!A1" xr:uid="{F2C1BDE2-DD5F-405D-AD25-06F570BAE0AB}"/>
-    <hyperlink ref="A9" r:id="rId8" location="CreateResWithOverridenRate!A1" xr:uid="{8103CA66-C07A-4BB4-BEF1-F221794D9D5D}"/>
-    <hyperlink ref="A10" r:id="rId9" location="CheckInWithZeroBalance!A1" xr:uid="{99859B79-BAD6-4CA7-AC9F-9B31D3B832DF}"/>
-    <hyperlink ref="A11" r:id="rId10" location="CheckoutWithZeroBalance!A1" xr:uid="{D487C994-47F0-4146-9C9D-6DCB438C8C18}"/>
-    <hyperlink ref="A12" r:id="rId11" location="VerifyResetOption!A1" xr:uid="{7BF7F122-C023-41C6-A41B-BC53F9D72884}"/>
-    <hyperlink ref="A13" r:id="rId12" location="GuestHistoryAccount!A1" xr:uid="{90272894-1C3F-4C44-8558-997009242CE2}"/>
-    <hyperlink ref="A14" r:id="rId13" location="GuestHistoryReservation!A1" xr:uid="{2F543DA4-450B-4403-89CE-E96553FCC566}"/>
-    <hyperlink ref="A15" r:id="rId14" location="AssociateResWithGuestHistory!A1" xr:uid="{33CE53E2-8A45-4FF8-8D88-25694F419209}"/>
-    <hyperlink ref="A16" r:id="rId15" location="FolioLineItemsVoid!A1" xr:uid="{1161EA33-5DBE-40CB-B002-431EBD43B1A3}"/>
-    <hyperlink ref="A17" r:id="rId16" location="LockUnlockFunctionality!A1" xr:uid="{CAECDCE0-5B99-4D06-83F8-21EDA208E9B1}"/>
-    <hyperlink ref="A18" r:id="rId17" location="Copy_Unassigned_Reservation!A1" xr:uid="{BA0B3315-14AD-4D06-8ACE-DCC6AB112D35}"/>
-    <hyperlink ref="A19" r:id="rId18" location="CopyReservationAssigned!A1" xr:uid="{44231D36-12AE-4AF0-81BA-3A2EFC9D4F73}"/>
-    <hyperlink ref="A20" r:id="rId19" location="Reservation_PromoCode!A1" xr:uid="{AB8295B4-3B4A-4D91-B3E5-3076F1B359B9}"/>
-    <hyperlink ref="A21" r:id="rId20" location="Reservation_With_NonRackRate!A1" xr:uid="{A2348F57-A964-46EB-B4C4-4F8095B3F785}"/>
-    <hyperlink ref="A22" r:id="rId21" location="PostLineItem!A1" xr:uid="{2630D8FD-F1EB-43E0-BA7B-CEB38327B2EF}"/>
-    <hyperlink ref="A23" r:id="rId22" location="BaseRate!A1" xr:uid="{033AB562-348D-45D1-A77F-D8BD9828DD3C}"/>
-    <hyperlink ref="A24" r:id="rId23" location="DerivedRate!A1" xr:uid="{4A2D94D4-6430-497E-8290-FD8D971A8549}"/>
-    <hyperlink ref="A25" r:id="rId24" location="PackageRate!A1" xr:uid="{51493BC1-B978-41F4-AD11-DAA2CF2C0636}"/>
-    <hyperlink ref="A26" r:id="rId25" location="SourceDefaultStatus!A1" xr:uid="{9EBC6879-5568-4FF6-9779-E497BED4715E}"/>
-    <hyperlink ref="A27" r:id="rId26" location="CreateRule!A1" xr:uid="{6BD13BF0-C090-4823-BC0E-6B3F0BB7B5B8}"/>
-    <hyperlink ref="A28" r:id="rId27" location="'New Edit Delete Folio'!A1" xr:uid="{44090C42-3935-441F-8B20-18CA2868FDEB}"/>
-    <hyperlink ref="A29" r:id="rId28" location="'Reservation with Split Rooms'!A1" xr:uid="{E614E026-237C-4A99-BD19-E6E03C8A3DC8}"/>
-    <hyperlink ref="A30" r:id="rId29" location="'Taxes and Tax Exempt'!A1" xr:uid="{3F850A4F-9863-4494-9F37-240D962A4A01}"/>
-    <hyperlink ref="A31" r:id="rId30" location="RateQuote_Book_Quote!A1" xr:uid="{14C7883A-32A5-4493-8D06-BD98D5FB9139}"/>
-    <hyperlink ref="A32" r:id="rId31" location="RateQuote_Book_Reservation!A1" xr:uid="{D4297ACA-BE87-4618-A870-155AE90CA388}"/>
+    <hyperlink ref="A2" r:id="rId1" location="Clean_Room_Classes!A1"/>
+    <hyperlink ref="A3" r:id="rId2" location="Delete_Reservation!A1"/>
+    <hyperlink ref="A4" r:id="rId3" location="Create_New_Policy!A1"/>
+    <hyperlink ref="A5" r:id="rId4" location="RetainPaymentInfoAfterEdit!A1"/>
+    <hyperlink ref="A6" r:id="rId5" location="VerifyItemDetail!A1"/>
+    <hyperlink ref="A7" r:id="rId6" location="VerifySaveBtnFuncForReservation!A1"/>
+    <hyperlink ref="A8" r:id="rId7" location="VerifySaveBtnFuncForAccounts!A1"/>
+    <hyperlink ref="A9" r:id="rId8" location="CreateResWithOverridenRate!A1"/>
+    <hyperlink ref="A10" r:id="rId9" location="CheckInWithZeroBalance!A1"/>
+    <hyperlink ref="A11" r:id="rId10" location="CheckoutWithZeroBalance!A1"/>
+    <hyperlink ref="A12" r:id="rId11" location="VerifyResetOption!A1"/>
+    <hyperlink ref="A13" r:id="rId12" location="GuestHistoryAccount!A1"/>
+    <hyperlink ref="A14" r:id="rId13" location="GuestHistoryReservation!A1"/>
+    <hyperlink ref="A15" r:id="rId14" location="AssociateResWithGuestHistory!A1"/>
+    <hyperlink ref="A16" r:id="rId15" location="FolioLineItemsVoid!A1"/>
+    <hyperlink ref="A17" r:id="rId16" location="LockUnlockFunctionality!A1"/>
+    <hyperlink ref="A18" r:id="rId17" location="Copy_Unassigned_Reservation!A1"/>
+    <hyperlink ref="A19" r:id="rId18" location="CopyReservationAssigned!A1"/>
+    <hyperlink ref="A20" r:id="rId19" location="Reservation_PromoCode!A1"/>
+    <hyperlink ref="A21" r:id="rId20" location="Reservation_With_NonRackRate!A1"/>
+    <hyperlink ref="A22" r:id="rId21" location="PostLineItem!A1"/>
+    <hyperlink ref="A23" r:id="rId22" location="BaseRate!A1"/>
+    <hyperlink ref="A24" r:id="rId23" location="DerivedRate!A1"/>
+    <hyperlink ref="A25" r:id="rId24" location="PackageRate!A1"/>
+    <hyperlink ref="A26" r:id="rId25" location="SourceDefaultStatus!A1"/>
+    <hyperlink ref="A27" r:id="rId26" location="CreateRule!A1"/>
+    <hyperlink ref="A28" r:id="rId27" location="'New Edit Delete Folio'!A1"/>
+    <hyperlink ref="A29" r:id="rId28" location="'Reservation with Split Rooms'!A1"/>
+    <hyperlink ref="A30" r:id="rId29" location="'Taxes and Tax Exempt'!A1"/>
+    <hyperlink ref="A31" r:id="rId30" location="RateQuote_Book_Quote!A1"/>
+    <hyperlink ref="A32" r:id="rId31" location="RateQuote_Book_Reservation!A1"/>
+    <hyperlink ref="A33" r:id="rId32" location="'Account Cash Payment'!A1"/>
+    <hyperlink ref="A34" r:id="rId33" location="AccountSearch!A1"/>
+    <hyperlink ref="A35" r:id="rId34" location="AssociateAccountToReservation!A1"/>
+    <hyperlink ref="A36" r:id="rId35" location="Ageing_ItemLeavel!A1"/>
+    <hyperlink ref="A37" r:id="rId36" location="Ageing_AutoApply!A1"/>
+    <hyperlink ref="A38" r:id="rId37" location="Ageing_AdvanceDeposit!A1"/>
+    <hyperlink ref="A39" r:id="rId38" location="'Move Folio'!A1"/>
+    <hyperlink ref="A40" r:id="rId39" location="'Move Folio Accross Reservations'!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2192,7 +2296,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2482,10 +2586,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN2" xr:uid="{00000000-0002-0000-0B00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{00000000-0002-0000-0B00-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
       <formula1>"Authorization Only,Capture,Credit"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2495,7 +2599,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2799,7 +2903,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2" xr:uid="{00000000-0002-0000-0C00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2809,7 +2913,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3113,7 +3217,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2" xr:uid="{00000000-0002-0000-0D00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3123,7 +3227,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3394,7 +3498,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2" xr:uid="{00000000-0002-0000-0E00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3404,7 +3508,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3709,7 +3813,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3988,7 +4092,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{00000000-0002-0000-1000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3998,7 +4102,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4089,7 +4193,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4159,7 +4263,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BP2"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
@@ -4629,13 +4733,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW2" xr:uid="{00000000-0002-0000-1300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW2">
       <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BC2" xr:uid="{00000000-0002-0000-1300-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BC2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB2" xr:uid="{00000000-0002-0000-1300-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB2">
       <formula1>"Authorization Only,Capture,Credit"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4644,7 +4748,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4973,10 +5077,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN2" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
       <formula1>"Authorization Only,Capture,Credit"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4986,7 +5090,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5311,13 +5415,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{00000000-0002-0000-1400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
       <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2" xr:uid="{00000000-0002-0000-1400-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2" xr:uid="{00000000-0002-0000-1400-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2">
       <formula1>"Authorization Only,Capture,Credit"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5326,7 +5430,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5651,13 +5755,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2" xr:uid="{00000000-0002-0000-1500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2">
       <formula1>"Authorization Only,Capture,Credit"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2" xr:uid="{00000000-0002-0000-1500-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{00000000-0002-0000-1500-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
       <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5666,7 +5770,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5991,13 +6095,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{00000000-0002-0000-1600-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
       <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2" xr:uid="{00000000-0002-0000-1600-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2" xr:uid="{00000000-0002-0000-1600-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2">
       <formula1>"Authorization Only,Capture,Credit"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6006,7 +6110,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6331,13 +6435,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2" xr:uid="{00000000-0002-0000-1700-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2">
       <formula1>"Authorization Only,Capture,Credit"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2" xr:uid="{00000000-0002-0000-1700-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{00000000-0002-0000-1700-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
       <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6346,7 +6450,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6696,10 +6800,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{00000000-0002-0000-1800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
       <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2" xr:uid="{00000000-0002-0000-1800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2">
       <formula1>"Authorization Only,Capture,Credit"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6708,7 +6812,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7042,13 +7146,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2" xr:uid="{00000000-0002-0000-1900-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2">
       <formula1>"Authorization Only,Capture,Credit"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{00000000-0002-0000-1900-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
       <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2" xr:uid="{00000000-0002-0000-1900-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7057,7 +7161,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7113,7 +7217,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7438,13 +7542,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{00000000-0002-0000-1B00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
       <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2" xr:uid="{00000000-0002-0000-1B00-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2" xr:uid="{00000000-0002-0000-1B00-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2">
       <formula1>"Authorization Only,Capture,Credit"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7453,7 +7557,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7676,13 +7780,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2" xr:uid="{00000000-0002-0000-1C00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2">
       <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2" xr:uid="{00000000-0002-0000-1C00-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2" xr:uid="{00000000-0002-0000-1C00-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2">
       <formula1>"Authorization Only,Capture,Credit"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7691,7 +7795,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F02DD7-07BD-41D4-99FE-CA76BE62A350}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7763,11 +7867,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7935,13 +8039,13 @@
         <v>157</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>89</v>
@@ -8023,7 +8127,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB7CB01-1DE5-4B85-93DF-1E4858E2A423}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8351,25 +8455,25 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{5C91B689-7C6F-47CB-93E6-519D3D539B8E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
       <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2" xr:uid="{1E45A798-7724-4601-9731-0D1F1C27131F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2" xr:uid="{5D9AFBAF-219E-413A-BECC-5FFD35CFD875}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2">
       <formula1>"Authorization Only,Capture,Credit"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="Test@147" xr:uid="{D0289F9E-9858-4090-AC00-6EC60C47434D}"/>
+    <hyperlink ref="D2" r:id="rId1" display="Test@147"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A63577FE-20D1-47A4-B306-8C5AB2318672}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8718,13 +8822,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2" xr:uid="{EC04F085-8F21-4EF7-9F97-A366F7419747}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2">
       <formula1>"Authorization Only,Capture,Credit"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2" xr:uid="{1518E516-7D0A-4B57-8DBF-8E0A6C1AA799}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{948FEBF6-C6BE-42C1-A147-D7FD68FAB67C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
       <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8733,7 +8837,7 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E123E7-838D-4A5A-BBB8-5B135524B148}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8983,7 +9087,7 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7389CE2F-8B6A-4593-A219-4A04EE24B362}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9311,13 +9415,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2" xr:uid="{56ED680C-D786-4FE6-84CC-26BE142EE13A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2">
       <formula1>"Authorization Only,Capture,Credit"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2" xr:uid="{0CCBDA98-645F-4095-B65B-73A3AF876DC4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{BE748F8B-88D0-4027-B242-1FA1BC7F030F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
       <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9326,7 +9430,7 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBA748A6-0C36-4D69-BA59-DE2D3BEFCB96}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9494,7 +9598,7 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264561A5-AADB-4864-AA72-47B3D68A2EDB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9703,7 +9807,7 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E84E1FF-B60B-4160-BBA0-5B88C8A1A342}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9761,7 +9865,7 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42062B5-DE24-4AEF-AB29-C84B958E2502}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9928,7 +10032,7 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E79D83D5-6C8B-48F1-8452-5830F6E0DF1A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10048,7 +10152,7 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB28894-3206-43A0-A9EB-083E62A1B046}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10140,7 +10244,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10202,7 +10306,7 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1A0BDE-061E-4A85-B4BD-6F7F56E9BDCC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10302,7 +10406,7 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B849E80-5CBD-48D5-BC5D-324AB1928966}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10581,7 +10685,7 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B8FD6F-0E78-4E06-B301-DAECEEC06A6A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10852,11 +10956,11 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18026C20-DC90-4AEB-9EB2-7A0C686A9C1B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11187,13 +11291,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2" xr:uid="{D3767A3B-AFB9-4D76-8DC6-46B596F0896E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2">
       <formula1>"Authorization Only,Capture,Credit"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AT2" xr:uid="{9BF68F37-474D-4F53-81DB-74D8F279BBF1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AT2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN2" xr:uid="{C0A505E9-F15A-42CD-B6DE-97779E87705B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN2">
       <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
     </dataValidation>
   </dataValidations>
@@ -11202,10 +11306,12 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEB5011A-6AED-4967-B96B-145143DB3360}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AB5" sqref="AB5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11437,7 +11543,7 @@
         <v>53</v>
       </c>
       <c r="AE2" s="15" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="AF2" s="15" t="s">
         <v>13</v>
@@ -11461,11 +11567,11 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861BCB79-5846-4A4D-B2C2-F554BC4C51DE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11588,7 +11694,7 @@
         <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>162</v>
+        <v>359</v>
       </c>
       <c r="H2" t="s">
         <v>53</v>
@@ -11648,11 +11754,11 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D230759-F1B0-4512-90E8-D91918F85654}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11803,7 +11909,7 @@
         <v>162</v>
       </c>
       <c r="H2" t="s">
-        <v>53</v>
+        <v>359</v>
       </c>
       <c r="I2" t="s">
         <v>53</v>
@@ -11836,7 +11942,7 @@
         <v>111</v>
       </c>
       <c r="S2" s="15" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="T2" s="15" t="s">
         <v>13</v>
@@ -11878,11 +11984,11 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B980F054-6051-4424-9C52-CB8797D166D6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12050,7 +12156,7 @@
         <v>157</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>101</v>
@@ -12137,93 +12243,8 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF819035-ACE0-420E-A08E-93CDB290F536}">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="Test@147" xr:uid="{B233DF8A-0D88-4F9F-A724-D4C6618B06F9}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419F7035-C6A3-4A85-AA18-044C3DEDD61A}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
@@ -12236,11 +12257,12 @@
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -12260,10 +12282,55 @@
         <v>72</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>48</v>
+        <v>333</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>158</v>
       </c>
@@ -12273,24 +12340,223 @@
       <c r="C2" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F2" s="24"/>
+      <c r="E2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>360</v>
+      </c>
       <c r="G2" s="3" t="s">
-        <v>335</v>
+        <v>243</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>340</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="Test@147"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>340</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12513,13 +12779,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2">
       <formula1>"Authorization Only,Capture,Credit"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2" xr:uid="{00000000-0002-0000-0400-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2" xr:uid="{00000000-0002-0000-0400-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2">
       <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
     </dataValidation>
   </dataValidations>
@@ -12529,11 +12795,11 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9FA1FF-DA15-4F28-B4A3-326C05CECB5D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12760,7 +13026,7 @@
         <v>53</v>
       </c>
       <c r="AE2" s="15" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="AF2" s="15" t="s">
         <v>13</v>
@@ -12778,11 +13044,11 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90DFCFB8-E961-437F-9FF4-A1FDB1F12867}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12791,12 +13057,11 @@
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -12809,18 +13074,71 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>336</v>
+      <c r="E1" s="1" t="s">
+        <v>309</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="H1" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>158</v>
       </c>
@@ -12833,16 +13151,69 @@
       <c r="D2" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>164</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12850,11 +13221,11 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF558AF-81A7-4EC8-A42E-D3D1FB7A665E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12928,7 +13299,7 @@
         <v>77</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>79</v>
@@ -12990,10 +13361,10 @@
         <v>161</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>11</v>
@@ -13002,31 +13373,31 @@
         <v>18</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>34</v>
@@ -13035,7 +13406,7 @@
         <v>317</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="U2" s="3" t="s">
         <v>119</v>
@@ -13044,7 +13415,7 @@
         <v>47</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="X2" s="3" t="s">
         <v>49</v>
@@ -13071,11 +13442,11 @@
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AD4E4A-FDA4-41F1-8A58-9CA501654EF5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13149,7 +13520,7 @@
         <v>77</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>79</v>
@@ -13211,10 +13582,10 @@
         <v>161</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>340</v>
+        <v>357</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>11</v>
@@ -13223,31 +13594,31 @@
         <v>18</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>34</v>
@@ -13256,7 +13627,7 @@
         <v>317</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="U2" s="3" t="s">
         <v>119</v>
@@ -13265,7 +13636,7 @@
         <v>47</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="X2" s="3" t="s">
         <v>49</v>
@@ -13292,11 +13663,11 @@
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75820A7E-CA40-44C2-A628-2758C34AE2F5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13370,7 +13741,7 @@
         <v>77</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>79</v>
@@ -13435,7 +13806,7 @@
         <v>82</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>340</v>
+        <v>356</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>11</v>
@@ -13444,31 +13815,31 @@
         <v>18</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>34</v>
@@ -13477,7 +13848,7 @@
         <v>317</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="U2" s="3" t="s">
         <v>119</v>
@@ -13486,7 +13857,7 @@
         <v>155</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="X2" s="3" t="s">
         <v>49</v>
@@ -13512,8 +13883,171 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="Test@147"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13837,10 +14371,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
       <formula1>"Authorization Only,Capture,Credit"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN2" xr:uid="{00000000-0002-0000-0500-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -13850,7 +14384,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14060,7 +14594,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14391,7 +14925,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -14401,7 +14935,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14691,10 +15225,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
       <formula1>"Authorization Only,Capture,Credit"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN2" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN2">
       <formula1>"Yes,NO"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Completed Bulk Checkin with zero balance along with bulk now show
</commit_message>
<xml_diff>
--- a/test-data/TestData.xlsx
+++ b/test-data/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vishali\inncenter.nextgen.automation\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1F10C5-2C2E-4C7F-9963-E9F6A4D6D3A4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94875E3-BAFF-4B1F-998F-88124A5A06E0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" firstSheet="27" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" firstSheet="27" activeTab="32" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testcases" sheetId="1" r:id="rId1"/>
@@ -43,37 +43,40 @@
     <sheet name="VerifySaveBtnFuncForAccounts" sheetId="51" r:id="rId28"/>
     <sheet name="CreateRule" sheetId="52" r:id="rId29"/>
     <sheet name="BulkCancellation" sheetId="89" r:id="rId30"/>
-    <sheet name="Copy_Unassigned_Reservation" sheetId="83" r:id="rId31"/>
-    <sheet name="FolioLineItemsVoid" sheetId="79" r:id="rId32"/>
-    <sheet name="Reservation_PromoCode" sheetId="55" r:id="rId33"/>
-    <sheet name="CopyReservationAssigned" sheetId="56" r:id="rId34"/>
-    <sheet name="GuestHistoryAccount" sheetId="82" r:id="rId35"/>
-    <sheet name="GuestHistoryReservation" sheetId="81" r:id="rId36"/>
-    <sheet name="LockUnlockFunctionality" sheetId="59" r:id="rId37"/>
-    <sheet name="AssociateResWithGuestHistory" sheetId="60" r:id="rId38"/>
-    <sheet name="BaseRate" sheetId="61" r:id="rId39"/>
-    <sheet name="DerivedRate" sheetId="62" r:id="rId40"/>
-    <sheet name="PackageRate" sheetId="63" r:id="rId41"/>
-    <sheet name="SourceDefaultStatus" sheetId="64" r:id="rId42"/>
-    <sheet name="Reservation_With_NonRackRate" sheetId="65" r:id="rId43"/>
-    <sheet name="PostLineItem" sheetId="80" r:id="rId44"/>
-    <sheet name="New Edit Delete Folio" sheetId="67" r:id="rId45"/>
-    <sheet name="Reservation with Split Rooms" sheetId="68" r:id="rId46"/>
-    <sheet name="Taxes and Tax Exempt" sheetId="69" r:id="rId47"/>
-    <sheet name="RateQuote_Book_Quote" sheetId="70" r:id="rId48"/>
-    <sheet name="Account Cash Payment" sheetId="71" r:id="rId49"/>
-    <sheet name="AccountSearch" sheetId="72" r:id="rId50"/>
-    <sheet name="AssociateAccountToReservation" sheetId="73" r:id="rId51"/>
-    <sheet name="Move Folio" sheetId="74" r:id="rId52"/>
-    <sheet name="Ageing_AdvanceDeposit" sheetId="75" r:id="rId53"/>
-    <sheet name="Ageing_AutoApply" sheetId="76" r:id="rId54"/>
-    <sheet name="Ageing_ItemLeavel" sheetId="77" r:id="rId55"/>
-    <sheet name="Move Folio Accross Reservations" sheetId="78" r:id="rId56"/>
-    <sheet name="Create_Corporate_Acc" sheetId="84" r:id="rId57"/>
-    <sheet name="Create_TravelAgent_Account" sheetId="85" r:id="rId58"/>
-    <sheet name="Create_Unitowner_Account" sheetId="86" r:id="rId59"/>
-    <sheet name="VerifyCashPayInRes" sheetId="87" r:id="rId60"/>
-    <sheet name="CopyReservation" sheetId="88" r:id="rId61"/>
+    <sheet name="BulkCancel" sheetId="90" r:id="rId31"/>
+    <sheet name="BulkNoShow" sheetId="91" r:id="rId32"/>
+    <sheet name="BulkCheckInWithZeroBalance" sheetId="92" r:id="rId33"/>
+    <sheet name="Copy_Unassigned_Reservation" sheetId="83" r:id="rId34"/>
+    <sheet name="FolioLineItemsVoid" sheetId="79" r:id="rId35"/>
+    <sheet name="Reservation_PromoCode" sheetId="55" r:id="rId36"/>
+    <sheet name="CopyReservationAssigned" sheetId="56" r:id="rId37"/>
+    <sheet name="GuestHistoryAccount" sheetId="82" r:id="rId38"/>
+    <sheet name="GuestHistoryReservation" sheetId="81" r:id="rId39"/>
+    <sheet name="LockUnlockFunctionality" sheetId="59" r:id="rId40"/>
+    <sheet name="AssociateResWithGuestHistory" sheetId="60" r:id="rId41"/>
+    <sheet name="BaseRate" sheetId="61" r:id="rId42"/>
+    <sheet name="DerivedRate" sheetId="62" r:id="rId43"/>
+    <sheet name="PackageRate" sheetId="63" r:id="rId44"/>
+    <sheet name="SourceDefaultStatus" sheetId="64" r:id="rId45"/>
+    <sheet name="Reservation_With_NonRackRate" sheetId="65" r:id="rId46"/>
+    <sheet name="PostLineItem" sheetId="80" r:id="rId47"/>
+    <sheet name="New Edit Delete Folio" sheetId="67" r:id="rId48"/>
+    <sheet name="Reservation with Split Rooms" sheetId="68" r:id="rId49"/>
+    <sheet name="Taxes and Tax Exempt" sheetId="69" r:id="rId50"/>
+    <sheet name="RateQuote_Book_Quote" sheetId="70" r:id="rId51"/>
+    <sheet name="Account Cash Payment" sheetId="71" r:id="rId52"/>
+    <sheet name="AccountSearch" sheetId="72" r:id="rId53"/>
+    <sheet name="AssociateAccountToReservation" sheetId="73" r:id="rId54"/>
+    <sheet name="Move Folio" sheetId="74" r:id="rId55"/>
+    <sheet name="Ageing_AdvanceDeposit" sheetId="75" r:id="rId56"/>
+    <sheet name="Ageing_AutoApply" sheetId="76" r:id="rId57"/>
+    <sheet name="Ageing_ItemLeavel" sheetId="77" r:id="rId58"/>
+    <sheet name="Move Folio Accross Reservations" sheetId="78" r:id="rId59"/>
+    <sheet name="Create_Corporate_Acc" sheetId="84" r:id="rId60"/>
+    <sheet name="Create_TravelAgent_Account" sheetId="85" r:id="rId61"/>
+    <sheet name="Create_Unitowner_Account" sheetId="86" r:id="rId62"/>
+    <sheet name="VerifyCashPayInRes" sheetId="87" r:id="rId63"/>
+    <sheet name="CopyReservation" sheetId="88" r:id="rId64"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -85,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3876" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4138" uniqueCount="398">
   <si>
     <t>test_name</t>
   </si>
@@ -1270,6 +1273,15 @@
   </si>
   <si>
     <t>BulkCancellation</t>
+  </si>
+  <si>
+    <t>BulkCancel</t>
+  </si>
+  <si>
+    <t>BulkNoShow</t>
+  </si>
+  <si>
+    <t>BulkCheckInWithZeroBalance</t>
   </si>
 </sst>
 </file>
@@ -1780,10 +1792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2011,35 +2023,37 @@
       <c r="A28" s="24" t="s">
         <v>394</v>
       </c>
-      <c r="B28" s="21"/>
+      <c r="B28" s="21" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="30" t="s">
-        <v>342</v>
-      </c>
-      <c r="B29" s="2" t="s">
+      <c r="A29" s="24" t="s">
+        <v>395</v>
+      </c>
+      <c r="B29" s="21" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
-        <v>343</v>
-      </c>
-      <c r="B30" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B30" s="21" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
-        <v>344</v>
-      </c>
-      <c r="B31" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B31" s="21" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
-        <v>345</v>
+      <c r="A32" s="30" t="s">
+        <v>342</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>5</v>
@@ -2047,39 +2061,39 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="31" t="s">
-        <v>347</v>
-      </c>
-      <c r="B34" s="5" t="s">
+      <c r="A34" s="24" t="s">
+        <v>344</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="31" t="s">
-        <v>348</v>
-      </c>
-      <c r="B35" s="5" t="s">
+      <c r="A35" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="31" t="s">
-        <v>349</v>
-      </c>
-      <c r="B36" s="5" t="s">
+      <c r="A36" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>5</v>
@@ -2087,7 +2101,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>5</v>
@@ -2095,7 +2109,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>5</v>
@@ -2103,7 +2117,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>5</v>
@@ -2111,47 +2125,47 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="34" t="s">
-        <v>364</v>
-      </c>
-      <c r="B42" s="35" t="s">
+      <c r="A42" s="31" t="s">
+        <v>352</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="16" t="s">
-        <v>372</v>
-      </c>
-      <c r="B43" s="2" t="s">
+      <c r="A43" s="31" t="s">
+        <v>353</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="24" t="s">
-        <v>373</v>
-      </c>
-      <c r="B44" s="2" t="s">
+      <c r="A44" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="24" t="s">
-        <v>374</v>
-      </c>
-      <c r="B45" s="2" t="s">
+      <c r="A45" s="34" t="s">
+        <v>364</v>
+      </c>
+      <c r="B45" s="35" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="24" t="s">
-        <v>375</v>
+      <c r="A46" s="16" t="s">
+        <v>372</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>5</v>
@@ -2159,9 +2173,33 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="24" t="s">
+        <v>373</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="24" t="s">
+        <v>374</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="24" t="s">
+        <v>375</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2193,25 +2231,28 @@
     <hyperlink ref="A25" r:id="rId24" location="PackageRate!A1" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
     <hyperlink ref="A26" r:id="rId25" location="SourceDefaultStatus!A1" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
     <hyperlink ref="A27" r:id="rId26" location="CreateRule!A1" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="A29" r:id="rId27" location="'New Edit Delete Folio'!A1" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="A30" r:id="rId28" location="'Reservation with Split Rooms'!A1" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="A31" r:id="rId29" location="'Taxes and Tax Exempt'!A1" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="A32" r:id="rId30" location="RateQuote_Book_Quote!A1" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="A33" r:id="rId31" location="RateQuote_Book_Reservation!A1" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="A34" r:id="rId32" location="'Account Cash Payment'!A1" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="A35" r:id="rId33" location="AccountSearch!A1" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="A36" r:id="rId34" location="AssociateAccountToReservation!A1" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="A37" r:id="rId35" location="Ageing_ItemLeavel!A1" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="A38" r:id="rId36" location="Ageing_AutoApply!A1" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="A39" r:id="rId37" location="Ageing_AdvanceDeposit!A1" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="A40" r:id="rId38" location="'Move Folio'!A1" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="A41" r:id="rId39" location="'Move Folio Accross Reservations'!A1" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="A42" r:id="rId40" location="Res_Acc_Policy_Verification!A1" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="A43" r:id="rId41" location="Create_Corporate_Acc!A1" xr:uid="{76306D56-7977-42BD-A7D8-15BB4E4E1F90}"/>
-    <hyperlink ref="A44" r:id="rId42" location="Create_TravelAgent_Account!A1" xr:uid="{C9DF76E8-AD02-45EC-B6ED-E1D6277BB0A4}"/>
-    <hyperlink ref="A45" r:id="rId43" location="Create_Unitowner_Account!A1" xr:uid="{CA38BF95-6320-4C8A-A2A5-4CB1F7A821B4}"/>
-    <hyperlink ref="A46" r:id="rId44" location="VerifyCashPayInRes!A1" xr:uid="{B42FAF17-8020-496B-94A7-B5F9CFA76F53}"/>
-    <hyperlink ref="A47" r:id="rId45" location="CopyReservation!A1" xr:uid="{362D2F70-A8D8-46C1-B33A-FD5A38B6840B}"/>
+    <hyperlink ref="A32" r:id="rId27" location="'New Edit Delete Folio'!A1" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="A33" r:id="rId28" location="'Reservation with Split Rooms'!A1" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="A34" r:id="rId29" location="'Taxes and Tax Exempt'!A1" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="A35" r:id="rId30" location="RateQuote_Book_Quote!A1" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="A36" r:id="rId31" location="RateQuote_Book_Reservation!A1" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="A37" r:id="rId32" location="'Account Cash Payment'!A1" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="A38" r:id="rId33" location="AccountSearch!A1" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="A39" r:id="rId34" location="AssociateAccountToReservation!A1" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="A40" r:id="rId35" location="Ageing_ItemLeavel!A1" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="A41" r:id="rId36" location="Ageing_AutoApply!A1" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="A42" r:id="rId37" location="Ageing_AdvanceDeposit!A1" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="A43" r:id="rId38" location="'Move Folio'!A1" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="A44" r:id="rId39" location="'Move Folio Accross Reservations'!A1" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="A45" r:id="rId40" location="Res_Acc_Policy_Verification!A1" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="A46" r:id="rId41" location="Create_Corporate_Acc!A1" xr:uid="{76306D56-7977-42BD-A7D8-15BB4E4E1F90}"/>
+    <hyperlink ref="A47" r:id="rId42" location="Create_TravelAgent_Account!A1" xr:uid="{C9DF76E8-AD02-45EC-B6ED-E1D6277BB0A4}"/>
+    <hyperlink ref="A48" r:id="rId43" location="Create_Unitowner_Account!A1" xr:uid="{CA38BF95-6320-4C8A-A2A5-4CB1F7A821B4}"/>
+    <hyperlink ref="A49" r:id="rId44" location="VerifyCashPayInRes!A1" xr:uid="{B42FAF17-8020-496B-94A7-B5F9CFA76F53}"/>
+    <hyperlink ref="A50" r:id="rId45" location="CopyReservation!A1" xr:uid="{362D2F70-A8D8-46C1-B33A-FD5A38B6840B}"/>
+    <hyperlink ref="A29" r:id="rId46" location="BulkCancel!A1" xr:uid="{58A38AD7-4935-487F-949D-67F77CD6352B}"/>
+    <hyperlink ref="A28" r:id="rId47" location="BulkCancellation!A1" xr:uid="{63EF7994-D3CF-4F37-BB0B-3BF5CF3C4AC3}"/>
+    <hyperlink ref="A30" r:id="rId48" location="BulkNoShow!A1" xr:uid="{FA09C011-53FD-45E4-AAF2-AFAD7CEC0D88}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6008,8 +6049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView topLeftCell="AL1" workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AZ2" sqref="AZ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8652,9 +8693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{300F3C78-0F33-4ED4-9449-D56166135341}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8698,11 +8737,910 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4035791-35D9-403F-B8DB-6AC05B7E1A51}">
+  <dimension ref="A1:AU2"/>
+  <sheetViews>
+    <sheetView topLeftCell="AE1" workbookViewId="0">
+      <selection sqref="A1:AU2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA1" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB1" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC1" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE1" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG1" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH1" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI1" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ1" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK1" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL1" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM1" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN1" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="AO1" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP1" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ1" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="AR1" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="AS1" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="AT1" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="AU1" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="T2" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="U2" s="17"/>
+      <c r="V2" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="W2" s="17"/>
+      <c r="X2" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB2" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC2" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD2" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="AE2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF2" s="17"/>
+      <c r="AG2" s="17"/>
+      <c r="AH2" s="17"/>
+      <c r="AI2" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="AJ2" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="AK2" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="AL2" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM2" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="AN2" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="AO2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP2" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="AQ2" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="AR2" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="AS2" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="AT2" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="AU2" s="17"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{F31E6B1C-3FBC-4BE4-9E89-BD9BDADA2400}">
+      <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2" xr:uid="{7268810E-8C6A-4412-BDFD-57D97E656CE9}">
+      <formula1>"Yes,NO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2" xr:uid="{B69CF1CC-0390-48FC-B2CD-7E00FC7F97EF}">
+      <formula1>"Authorization Only,Capture,Credit"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="Test@147" xr:uid="{E4C169A1-CEB0-4187-B25B-FFC36BF05DE9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD53283-6979-4DF7-8783-3A1BE2FD041E}">
+  <dimension ref="A1:AU2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA1" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB1" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC1" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE1" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG1" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH1" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI1" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ1" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK1" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL1" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM1" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN1" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="AO1" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP1" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ1" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="AR1" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="AS1" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="AT1" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="AU1" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="T2" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="U2" s="17"/>
+      <c r="V2" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="W2" s="17"/>
+      <c r="X2" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB2" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC2" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD2" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="AE2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF2" s="17"/>
+      <c r="AG2" s="17"/>
+      <c r="AH2" s="17"/>
+      <c r="AI2" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="AJ2" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="AK2" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="AL2" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM2" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="AN2" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="AO2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP2" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="AQ2" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="AR2" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="AS2" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="AT2" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="AU2" s="17"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2" xr:uid="{F918D5A0-B1C3-4EE9-B3A7-F16425AF3739}">
+      <formula1>"Authorization Only,Capture,Credit"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2" xr:uid="{D6A9966C-FF70-4B3C-8A0E-2F783980F5AD}">
+      <formula1>"Yes,NO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{56856A74-7628-4213-A0A4-E54BCAD615AD}">
+      <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="Test@147" xr:uid="{846C5CB2-EB6C-4723-BBAE-92714F463877}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DD98410-B810-434A-AD0E-0C60B4B77F71}">
+  <dimension ref="A1:AU2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="U1" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA1" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB1" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC1" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE1" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG1" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH1" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI1" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ1" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK1" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL1" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM1" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN1" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="AO1" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP1" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ1" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="AR1" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="AS1" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="AT1" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="AU1" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="T2" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="U2" s="17"/>
+      <c r="V2" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="W2" s="17"/>
+      <c r="X2" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB2" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC2" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD2" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="AE2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF2" s="17"/>
+      <c r="AG2" s="17"/>
+      <c r="AH2" s="17"/>
+      <c r="AI2" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="AJ2" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="AK2" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="AL2" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM2" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="AN2" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="AO2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP2" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="AQ2" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="AR2" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="AS2" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="AT2" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="AU2" s="17"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{F7DA2CDA-F3EC-4A31-8772-71BDF4D5AD0C}">
+      <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2" xr:uid="{18E8DA6C-BCA1-4B28-B4A0-B255FB3C5FF2}">
+      <formula1>"Yes,NO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2" xr:uid="{34527731-12F3-4AD9-909C-8FC18D9C1F9B}">
+      <formula1>"Authorization Only,Capture,Credit"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="Test@147" xr:uid="{887B014B-252A-49AB-B96F-7DB44EDFC0BB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE605292-599F-4F8A-AAC7-A035595785AA}">
   <dimension ref="A1:AU41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AT11" sqref="AT11"/>
+      <selection sqref="A1:AU2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9047,7 +9985,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E2A777-D660-4E29-9A12-D4622C63C634}">
   <dimension ref="A1:BA2"/>
   <sheetViews>
@@ -9433,7 +10371,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
@@ -9683,7 +10621,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:AU2"/>
   <sheetViews>
@@ -10026,7 +10964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98005182-BDD5-463C-8DCE-0C0CB45FBDAC}">
   <dimension ref="A1:U2"/>
   <sheetViews>
@@ -10194,7 +11132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79DD2FC-1F8B-4668-946A-A1FDC237537B}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -10403,7 +11341,69 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -10461,7 +11461,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
@@ -10628,7 +11628,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -10748,69 +11748,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -10902,7 +11840,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -11002,7 +11940,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A1:AM2"/>
   <sheetViews>
@@ -11281,7 +12219,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
   <dimension ref="A1:AL2"/>
   <sheetViews>
@@ -11552,7 +12490,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00297B8D-6F4E-4ED6-9338-E4F11C979F8C}">
   <dimension ref="A1:AY2"/>
   <sheetViews>
@@ -11922,12 +12860,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AB5" sqref="AB5"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12183,7 +13121,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
   <dimension ref="A1:X2"/>
   <sheetViews>
@@ -12366,659 +13304,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
-  <dimension ref="A1:AD2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" t="s">
-        <v>312</v>
-      </c>
-      <c r="N1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O1" t="s">
-        <v>313</v>
-      </c>
-      <c r="P1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>314</v>
-      </c>
-      <c r="R1" t="s">
-        <v>315</v>
-      </c>
-      <c r="S1" t="s">
-        <v>54</v>
-      </c>
-      <c r="T1" t="s">
-        <v>308</v>
-      </c>
-      <c r="U1" t="s">
-        <v>55</v>
-      </c>
-      <c r="V1" t="s">
-        <v>61</v>
-      </c>
-      <c r="W1" t="s">
-        <v>57</v>
-      </c>
-      <c r="X1" t="s">
-        <v>322</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>323</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>324</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>325</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>326</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>327</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>162</v>
-      </c>
-      <c r="H2" t="s">
-        <v>359</v>
-      </c>
-      <c r="I2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" t="s">
-        <v>162</v>
-      </c>
-      <c r="K2" t="s">
-        <v>317</v>
-      </c>
-      <c r="L2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>318</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="O2" t="s">
-        <v>229</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>320</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>321</v>
-      </c>
-      <c r="R2" t="s">
-        <v>111</v>
-      </c>
-      <c r="S2" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="T2" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="U2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="V2" t="s">
-        <v>91</v>
-      </c>
-      <c r="W2" t="s">
-        <v>164</v>
-      </c>
-      <c r="X2" t="s">
-        <v>329</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>329</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>329</v>
-      </c>
-      <c r="AA2" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>330</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>331</v>
-      </c>
-      <c r="AD2">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
-  <dimension ref="A1:AJ2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AF1" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="S2" s="3">
-        <v>4889</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
-  <dimension ref="A1:V2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>336</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>340</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="Test@147" xr:uid="{00000000-0004-0000-2F00-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -13263,6 +13548,657 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
+  <dimension ref="A1:AD2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" t="s">
+        <v>312</v>
+      </c>
+      <c r="N1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" t="s">
+        <v>313</v>
+      </c>
+      <c r="P1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>314</v>
+      </c>
+      <c r="R1" t="s">
+        <v>315</v>
+      </c>
+      <c r="S1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" t="s">
+        <v>308</v>
+      </c>
+      <c r="U1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" t="s">
+        <v>61</v>
+      </c>
+      <c r="W1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X1" t="s">
+        <v>322</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>323</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>324</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>325</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>326</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>327</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H2" t="s">
+        <v>359</v>
+      </c>
+      <c r="I2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" t="s">
+        <v>162</v>
+      </c>
+      <c r="K2" t="s">
+        <v>317</v>
+      </c>
+      <c r="L2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="O2" t="s">
+        <v>229</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>321</v>
+      </c>
+      <c r="R2" t="s">
+        <v>111</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="V2" t="s">
+        <v>91</v>
+      </c>
+      <c r="W2" t="s">
+        <v>164</v>
+      </c>
+      <c r="X2" t="s">
+        <v>329</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>329</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>329</v>
+      </c>
+      <c r="AA2" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>330</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>331</v>
+      </c>
+      <c r="AD2">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
+  <dimension ref="A1:AJ2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" s="3">
+        <v>4889</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
+  <dimension ref="A1:V2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>340</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="Test@147" xr:uid="{00000000-0004-0000-2F00-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
@@ -13411,13 +14347,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AA9" sqref="AA9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13660,12 +14594,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13837,7 +14771,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
@@ -14058,7 +14992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
@@ -14279,7 +15213,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
@@ -14500,7 +15434,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
@@ -14660,946 +15594,6 @@
     <hyperlink ref="D2" r:id="rId1" display="Test@147" xr:uid="{00000000-0004-0000-3600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656154C9-F525-4E04-BBB0-A63D4463202D}">
-  <dimension ref="A1:AO2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="AF1" s="38" t="s">
-        <v>378</v>
-      </c>
-      <c r="AG1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AH1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="AI1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN1" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH2" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="AI2" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="AM2" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="AN2" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="AO2" s="1"/>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2" xr:uid="{A30ECA5D-0F82-4F65-BBC6-CFF7F6BB9CA6}">
-      <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2" xr:uid="{D27DA2B4-7021-479E-A002-E047340FE88A}">
-      <formula1>"Yes,NO"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2" xr:uid="{D6BAEA79-02C4-4260-AEDD-0AFEB99AB26E}">
-      <formula1>"Authorization Only,Capture,Credit"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="Test@147" xr:uid="{55B3BB4D-00E3-4F8C-94A0-76AC98EC8EB9}"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://app.innroad.com/" xr:uid="{22706AD2-EC34-4122-B880-789D8BD21A90}"/>
-    <hyperlink ref="Q2" r:id="rId3" display="auto@gmail.com" xr:uid="{56752A12-9395-432F-A4F8-5FBC2027604B}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17D8CD14-F2B6-41FF-B860-BBB543ECE21E}">
-  <dimension ref="A1:AP2"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="8.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="AI2" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="AJ2" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="AN2" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="AO2" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="AP2" s="1"/>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2" xr:uid="{F278AEA8-3B93-481E-BFAB-3ED197136538}">
-      <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2" xr:uid="{96B5495B-FF8A-40AD-B7B8-F68FD574025E}">
-      <formula1>"Yes,NO"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2" xr:uid="{D8F4D6FD-B019-4008-B4D1-602C87A3D9D3}">
-      <formula1>"Authorization Only,Capture,Credit"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE3D6DD-6BE6-4EB6-B2A0-BD80FDA3D32F}">
-  <dimension ref="A1:AO2"/>
-  <sheetViews>
-    <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="AG1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AH1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="AI1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN1" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="AG2" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH2" s="39" t="s">
-        <v>169</v>
-      </c>
-      <c r="AI2" s="39" t="s">
-        <v>169</v>
-      </c>
-      <c r="AJ2" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="AL2" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="AM2" s="27" t="s">
-        <v>254</v>
-      </c>
-      <c r="AN2" s="27" t="s">
-        <v>101</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2" xr:uid="{BCAD8A34-AC2F-4C11-9D6B-29A439B4890A}">
-      <formula1>"Authorization Only,Capture,Credit"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2" xr:uid="{AD3634BB-EB9A-4A8E-9180-104344B54046}">
-      <formula1>"Yes,NO"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2" xr:uid="{C6CDF011-4267-467B-8C2F-6D95B7FE81D4}">
-      <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -15941,6 +15935,946 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656154C9-F525-4E04-BBB0-A63D4463202D}">
+  <dimension ref="A1:AO2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="AF1" s="38" t="s">
+        <v>378</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN1" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH2" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="AI2" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM2" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AO2" s="1"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2" xr:uid="{A30ECA5D-0F82-4F65-BBC6-CFF7F6BB9CA6}">
+      <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2" xr:uid="{D27DA2B4-7021-479E-A002-E047340FE88A}">
+      <formula1>"Yes,NO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2" xr:uid="{D6BAEA79-02C4-4260-AEDD-0AFEB99AB26E}">
+      <formula1>"Authorization Only,Capture,Credit"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="Test@147" xr:uid="{55B3BB4D-00E3-4F8C-94A0-76AC98EC8EB9}"/>
+    <hyperlink ref="A2" r:id="rId2" display="https://app.innroad.com/" xr:uid="{22706AD2-EC34-4122-B880-789D8BD21A90}"/>
+    <hyperlink ref="Q2" r:id="rId3" display="auto@gmail.com" xr:uid="{56752A12-9395-432F-A4F8-5FBC2027604B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17D8CD14-F2B6-41FF-B860-BBB543ECE21E}">
+  <dimension ref="A1:AP2"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="8.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI2" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="AJ2" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="AO2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AP2" s="1"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2" xr:uid="{F278AEA8-3B93-481E-BFAB-3ED197136538}">
+      <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2" xr:uid="{96B5495B-FF8A-40AD-B7B8-F68FD574025E}">
+      <formula1>"Yes,NO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2" xr:uid="{D8F4D6FD-B019-4008-B4D1-602C87A3D9D3}">
+      <formula1>"Authorization Only,Capture,Credit"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE3D6DD-6BE6-4EB6-B2A0-BD80FDA3D32F}">
+  <dimension ref="A1:AO2"/>
+  <sheetViews>
+    <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN1" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="AG2" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="AH2" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="AI2" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="AJ2" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL2" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM2" s="27" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN2" s="27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2" xr:uid="{BCAD8A34-AC2F-4C11-9D6B-29A439B4890A}">
+      <formula1>"Authorization Only,Capture,Credit"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2" xr:uid="{AD3634BB-EB9A-4A8E-9180-104344B54046}">
+      <formula1>"Yes,NO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2" xr:uid="{C6CDF011-4267-467B-8C2F-6D95B7FE81D4}">
+      <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6518BCCF-A49D-470B-A017-45C992076BFA}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
@@ -16178,7 +17112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B7CD056-C366-41D6-BA4E-5671FEB95BD6}">
   <dimension ref="A1:AC2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Modified test-data for AUTOMATION-76
</commit_message>
<xml_diff>
--- a/test-data/TestData.xlsx
+++ b/test-data/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vishali\inncenter.nextgen.automation\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E202CF-7792-496F-81BE-9918F8857CD1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8C6B2D-1549-409D-BDE5-31017B3C4BE8}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" firstSheet="28" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,37 +46,38 @@
     <sheet name="BulkCancel" sheetId="90" r:id="rId31"/>
     <sheet name="BulkNoShow" sheetId="91" r:id="rId32"/>
     <sheet name="BulkCheckInWithZeroBalance" sheetId="92" r:id="rId33"/>
-    <sheet name="Copy_Unassigned_Reservation" sheetId="83" r:id="rId34"/>
-    <sheet name="FolioLineItemsVoid" sheetId="79" r:id="rId35"/>
-    <sheet name="Reservation_PromoCode" sheetId="55" r:id="rId36"/>
-    <sheet name="CopyReservationAssigned" sheetId="56" r:id="rId37"/>
-    <sheet name="GuestHistoryAccount" sheetId="82" r:id="rId38"/>
-    <sheet name="GuestHistoryReservation" sheetId="81" r:id="rId39"/>
-    <sheet name="LockUnlockFunctionality" sheetId="59" r:id="rId40"/>
-    <sheet name="AssociateResWithGuestHistory" sheetId="60" r:id="rId41"/>
-    <sheet name="BaseRate" sheetId="61" r:id="rId42"/>
-    <sheet name="DerivedRate" sheetId="62" r:id="rId43"/>
-    <sheet name="PackageRate" sheetId="63" r:id="rId44"/>
-    <sheet name="SourceDefaultStatus" sheetId="64" r:id="rId45"/>
-    <sheet name="Reservation_With_NonRackRate" sheetId="65" r:id="rId46"/>
-    <sheet name="PostLineItem" sheetId="80" r:id="rId47"/>
-    <sheet name="New Edit Delete Folio" sheetId="67" r:id="rId48"/>
-    <sheet name="Reservation with Split Rooms" sheetId="68" r:id="rId49"/>
-    <sheet name="Taxes and Tax Exempt" sheetId="69" r:id="rId50"/>
-    <sheet name="RateQuote_Book_Quote" sheetId="70" r:id="rId51"/>
-    <sheet name="Account Cash Payment" sheetId="71" r:id="rId52"/>
-    <sheet name="AccountSearch" sheetId="72" r:id="rId53"/>
-    <sheet name="AssociateAccountToReservation" sheetId="73" r:id="rId54"/>
-    <sheet name="Move Folio" sheetId="74" r:id="rId55"/>
-    <sheet name="Ageing_AdvanceDeposit" sheetId="75" r:id="rId56"/>
-    <sheet name="Ageing_AutoApply" sheetId="76" r:id="rId57"/>
-    <sheet name="Ageing_ItemLeavel" sheetId="77" r:id="rId58"/>
-    <sheet name="Move Folio Accross Reservations" sheetId="78" r:id="rId59"/>
-    <sheet name="Create_Corporate_Acc" sheetId="84" r:id="rId60"/>
-    <sheet name="Create_TravelAgent_Account" sheetId="85" r:id="rId61"/>
-    <sheet name="Create_Unitowner_Account" sheetId="86" r:id="rId62"/>
-    <sheet name="VerifyCashPayInRes" sheetId="87" r:id="rId63"/>
-    <sheet name="CopyReservation" sheetId="88" r:id="rId64"/>
+    <sheet name="BulkCheckOutWithZeroBalance" sheetId="93" r:id="rId34"/>
+    <sheet name="Copy_Unassigned_Reservation" sheetId="83" r:id="rId35"/>
+    <sheet name="FolioLineItemsVoid" sheetId="79" r:id="rId36"/>
+    <sheet name="Reservation_PromoCode" sheetId="55" r:id="rId37"/>
+    <sheet name="CopyReservationAssigned" sheetId="56" r:id="rId38"/>
+    <sheet name="GuestHistoryAccount" sheetId="82" r:id="rId39"/>
+    <sheet name="GuestHistoryReservation" sheetId="81" r:id="rId40"/>
+    <sheet name="LockUnlockFunctionality" sheetId="59" r:id="rId41"/>
+    <sheet name="AssociateResWithGuestHistory" sheetId="60" r:id="rId42"/>
+    <sheet name="BaseRate" sheetId="61" r:id="rId43"/>
+    <sheet name="DerivedRate" sheetId="62" r:id="rId44"/>
+    <sheet name="PackageRate" sheetId="63" r:id="rId45"/>
+    <sheet name="SourceDefaultStatus" sheetId="64" r:id="rId46"/>
+    <sheet name="Reservation_With_NonRackRate" sheetId="65" r:id="rId47"/>
+    <sheet name="PostLineItem" sheetId="80" r:id="rId48"/>
+    <sheet name="New Edit Delete Folio" sheetId="67" r:id="rId49"/>
+    <sheet name="Reservation with Split Rooms" sheetId="68" r:id="rId50"/>
+    <sheet name="Taxes and Tax Exempt" sheetId="69" r:id="rId51"/>
+    <sheet name="RateQuote_Book_Quote" sheetId="70" r:id="rId52"/>
+    <sheet name="Account Cash Payment" sheetId="71" r:id="rId53"/>
+    <sheet name="AccountSearch" sheetId="72" r:id="rId54"/>
+    <sheet name="AssociateAccountToReservation" sheetId="73" r:id="rId55"/>
+    <sheet name="Move Folio" sheetId="74" r:id="rId56"/>
+    <sheet name="Ageing_AdvanceDeposit" sheetId="75" r:id="rId57"/>
+    <sheet name="Ageing_AutoApply" sheetId="76" r:id="rId58"/>
+    <sheet name="Ageing_ItemLeavel" sheetId="77" r:id="rId59"/>
+    <sheet name="Move Folio Accross Reservations" sheetId="78" r:id="rId60"/>
+    <sheet name="Create_Corporate_Acc" sheetId="84" r:id="rId61"/>
+    <sheet name="Create_TravelAgent_Account" sheetId="85" r:id="rId62"/>
+    <sheet name="Create_Unitowner_Account" sheetId="86" r:id="rId63"/>
+    <sheet name="VerifyCashPayInRes" sheetId="87" r:id="rId64"/>
+    <sheet name="CopyReservation" sheetId="88" r:id="rId65"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -88,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4139" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4226" uniqueCount="399">
   <si>
     <t>test_name</t>
   </si>
@@ -1282,6 +1283,9 @@
   </si>
   <si>
     <t>BulkCheckInWithZeroBalance</t>
+  </si>
+  <si>
+    <t>BulkCheckOutWithZeroBalance</t>
   </si>
 </sst>
 </file>
@@ -1779,10 +1783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2039,16 +2043,14 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
-        <v>342</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="A32" s="24" t="s">
+        <v>398</v>
+      </c>
+      <c r="B32" s="21"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
-        <v>343</v>
+      <c r="A33" s="30" t="s">
+        <v>342</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>5</v>
@@ -2056,7 +2058,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>5</v>
@@ -2064,7 +2066,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>5</v>
@@ -2072,23 +2074,23 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="31" t="s">
-        <v>347</v>
-      </c>
-      <c r="B37" s="5" t="s">
+      <c r="A37" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>5</v>
@@ -2096,7 +2098,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>5</v>
@@ -2104,7 +2106,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>5</v>
@@ -2112,7 +2114,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>5</v>
@@ -2120,7 +2122,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>5</v>
@@ -2128,7 +2130,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>5</v>
@@ -2136,31 +2138,31 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="34" t="s">
-        <v>364</v>
-      </c>
-      <c r="B45" s="35" t="s">
+      <c r="A45" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="16" t="s">
-        <v>372</v>
-      </c>
-      <c r="B46" s="2" t="s">
+      <c r="A46" s="34" t="s">
+        <v>364</v>
+      </c>
+      <c r="B46" s="35" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="24" t="s">
-        <v>373</v>
+      <c r="A47" s="16" t="s">
+        <v>372</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>5</v>
@@ -2168,7 +2170,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="24" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>5</v>
@@ -2176,7 +2178,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="24" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>5</v>
@@ -2184,9 +2186,17 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
+        <v>375</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="24" t="s">
         <v>376</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2218,28 +2228,29 @@
     <hyperlink ref="A25" r:id="rId24" location="PackageRate!A1" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
     <hyperlink ref="A26" r:id="rId25" location="SourceDefaultStatus!A1" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
     <hyperlink ref="A27" r:id="rId26" location="CreateRule!A1" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="A32" r:id="rId27" location="'New Edit Delete Folio'!A1" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="A33" r:id="rId28" location="'Reservation with Split Rooms'!A1" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="A34" r:id="rId29" location="'Taxes and Tax Exempt'!A1" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="A35" r:id="rId30" location="RateQuote_Book_Quote!A1" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="A36" r:id="rId31" location="RateQuote_Book_Reservation!A1" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="A37" r:id="rId32" location="'Account Cash Payment'!A1" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="A38" r:id="rId33" location="AccountSearch!A1" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="A39" r:id="rId34" location="AssociateAccountToReservation!A1" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="A40" r:id="rId35" location="Ageing_ItemLeavel!A1" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="A41" r:id="rId36" location="Ageing_AutoApply!A1" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="A42" r:id="rId37" location="Ageing_AdvanceDeposit!A1" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="A43" r:id="rId38" location="'Move Folio'!A1" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="A44" r:id="rId39" location="'Move Folio Accross Reservations'!A1" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="A45" r:id="rId40" location="Res_Acc_Policy_Verification!A1" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="A46" r:id="rId41" location="Create_Corporate_Acc!A1" xr:uid="{76306D56-7977-42BD-A7D8-15BB4E4E1F90}"/>
-    <hyperlink ref="A47" r:id="rId42" location="Create_TravelAgent_Account!A1" xr:uid="{C9DF76E8-AD02-45EC-B6ED-E1D6277BB0A4}"/>
-    <hyperlink ref="A48" r:id="rId43" location="Create_Unitowner_Account!A1" xr:uid="{CA38BF95-6320-4C8A-A2A5-4CB1F7A821B4}"/>
-    <hyperlink ref="A49" r:id="rId44" location="VerifyCashPayInRes!A1" xr:uid="{B42FAF17-8020-496B-94A7-B5F9CFA76F53}"/>
-    <hyperlink ref="A50" r:id="rId45" location="CopyReservation!A1" xr:uid="{362D2F70-A8D8-46C1-B33A-FD5A38B6840B}"/>
+    <hyperlink ref="A33" r:id="rId27" location="'New Edit Delete Folio'!A1" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="A34" r:id="rId28" location="'Reservation with Split Rooms'!A1" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="A35" r:id="rId29" location="'Taxes and Tax Exempt'!A1" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="A36" r:id="rId30" location="RateQuote_Book_Quote!A1" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="A37" r:id="rId31" location="RateQuote_Book_Reservation!A1" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="A38" r:id="rId32" location="'Account Cash Payment'!A1" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="A39" r:id="rId33" location="AccountSearch!A1" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="A40" r:id="rId34" location="AssociateAccountToReservation!A1" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="A41" r:id="rId35" location="Ageing_ItemLeavel!A1" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="A42" r:id="rId36" location="Ageing_AutoApply!A1" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="A43" r:id="rId37" location="Ageing_AdvanceDeposit!A1" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="A44" r:id="rId38" location="'Move Folio'!A1" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="A45" r:id="rId39" location="'Move Folio Accross Reservations'!A1" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="A46" r:id="rId40" location="Res_Acc_Policy_Verification!A1" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="A47" r:id="rId41" location="Create_Corporate_Acc!A1" xr:uid="{76306D56-7977-42BD-A7D8-15BB4E4E1F90}"/>
+    <hyperlink ref="A48" r:id="rId42" location="Create_TravelAgent_Account!A1" xr:uid="{C9DF76E8-AD02-45EC-B6ED-E1D6277BB0A4}"/>
+    <hyperlink ref="A49" r:id="rId43" location="Create_Unitowner_Account!A1" xr:uid="{CA38BF95-6320-4C8A-A2A5-4CB1F7A821B4}"/>
+    <hyperlink ref="A50" r:id="rId44" location="VerifyCashPayInRes!A1" xr:uid="{B42FAF17-8020-496B-94A7-B5F9CFA76F53}"/>
+    <hyperlink ref="A51" r:id="rId45" location="CopyReservation!A1" xr:uid="{362D2F70-A8D8-46C1-B33A-FD5A38B6840B}"/>
     <hyperlink ref="A29" r:id="rId46" location="BulkCancel!A1" xr:uid="{58A38AD7-4935-487F-949D-67F77CD6352B}"/>
     <hyperlink ref="A28" r:id="rId47" location="BulkCancellation!A1" xr:uid="{63EF7994-D3CF-4F37-BB0B-3BF5CF3C4AC3}"/>
     <hyperlink ref="A30" r:id="rId48" location="BulkNoShow!A1" xr:uid="{FA09C011-53FD-45E4-AAF2-AFAD7CEC0D88}"/>
+    <hyperlink ref="A31" r:id="rId49" location="BulkCheckInWithZeroBalance!A1" xr:uid="{76EC9CF3-645B-4115-B53B-C943208BD34E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6036,9 +6047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AZ2" sqref="AZ2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9323,10 +9332,10 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DD98410-B810-434A-AD0E-0C60B4B77F71}">
-  <dimension ref="A1:AV2"/>
+  <dimension ref="A1:AU2"/>
   <sheetViews>
     <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="Z24" activeCellId="1" sqref="AB23 Z24"/>
+      <selection activeCell="U1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9334,7 +9343,7 @@
     <col min="1" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>6</v>
       </c>
@@ -9476,11 +9485,8 @@
       <c r="AU1" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="AV1" s="21" t="s">
-        <v>62</v>
-      </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>158</v>
       </c>
@@ -9604,7 +9610,6 @@
         <v>101</v>
       </c>
       <c r="AU2" s="17"/>
-      <c r="AV2" s="17"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -9627,11 +9632,312 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9323416-447E-48BB-AEE3-B779F20D4B9F}">
+  <dimension ref="A1:AV2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AV1" sqref="AV1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA1" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB1" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC1" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE1" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG1" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH1" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI1" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ1" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK1" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL1" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM1" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN1" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="AO1" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP1" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ1" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="AR1" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="AS1" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="AT1" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="AU1" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="AV1" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="T2" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="U2" s="17"/>
+      <c r="V2" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="W2" s="17"/>
+      <c r="X2" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB2" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC2" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD2" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="AE2" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF2" s="17"/>
+      <c r="AG2" s="17"/>
+      <c r="AH2" s="17"/>
+      <c r="AI2" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="AJ2" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="AK2" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="AL2" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="AM2" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="AN2" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="AO2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP2" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="AQ2" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="AR2" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="AS2" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="AT2" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="AU2" s="17"/>
+      <c r="AV2" s="17"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2" xr:uid="{9B356267-2833-4545-A125-639AB2ECD994}">
+      <formula1>"Authorization Only,Capture,Credit"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS2" xr:uid="{4DBFBBDB-E6FF-4696-A736-16BE0B32B266}">
+      <formula1>"Yes,NO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2" xr:uid="{B629ADE4-5042-49F3-B706-F0D1A1093BE2}">
+      <formula1>"Cash,MC,Check,Gift Certificate,House Account,Reservation"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="Test@147" xr:uid="{74E1754F-75F2-4370-AB37-4253BD5C4C72}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE605292-599F-4F8A-AAC7-A035595785AA}">
-  <dimension ref="A1:AU2"/>
+  <dimension ref="A1:AU32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9953,6 +10259,11 @@
       </c>
       <c r="AU2" s="17"/>
     </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
+        <v>398</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2" xr:uid="{79C60337-1B8D-44C6-84C3-86B6660CBFEE}">
@@ -9972,7 +10283,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35E2A777-D660-4E29-9A12-D4622C63C634}">
   <dimension ref="A1:BA2"/>
   <sheetViews>
@@ -10358,7 +10669,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
@@ -10608,7 +10919,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:AU2"/>
   <sheetViews>
@@ -10951,7 +11262,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98005182-BDD5-463C-8DCE-0C0CB45FBDAC}">
   <dimension ref="A1:U2"/>
   <sheetViews>
@@ -11119,7 +11430,69 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79DD2FC-1F8B-4668-946A-A1FDC237537B}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -11328,69 +11701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -11448,7 +11759,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
@@ -11615,7 +11926,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -11735,7 +12046,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -11827,7 +12138,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -11927,7 +12238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A1:AM2"/>
   <sheetViews>
@@ -12206,12 +12517,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
   <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12477,7 +12788,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00297B8D-6F4E-4ED6-9338-E4F11C979F8C}">
   <dimension ref="A1:AY2"/>
   <sheetViews>
@@ -12847,7 +13158,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
@@ -13108,193 +13419,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
-  <dimension ref="A1:X2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="17" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" t="s">
-        <v>312</v>
-      </c>
-      <c r="N1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O1" t="s">
-        <v>313</v>
-      </c>
-      <c r="P1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>314</v>
-      </c>
-      <c r="R1" t="s">
-        <v>315</v>
-      </c>
-      <c r="S1" t="s">
-        <v>54</v>
-      </c>
-      <c r="T1" t="s">
-        <v>308</v>
-      </c>
-      <c r="U1" t="s">
-        <v>55</v>
-      </c>
-      <c r="V1" t="s">
-        <v>61</v>
-      </c>
-      <c r="W1" t="s">
-        <v>57</v>
-      </c>
-      <c r="X1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>359</v>
-      </c>
-      <c r="H2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" t="s">
-        <v>162</v>
-      </c>
-      <c r="K2" t="s">
-        <v>317</v>
-      </c>
-      <c r="L2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>318</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="O2" t="s">
-        <v>229</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>320</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>321</v>
-      </c>
-      <c r="R2" t="s">
-        <v>111</v>
-      </c>
-      <c r="S2" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="T2" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="U2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="V2" t="s">
-        <v>91</v>
-      </c>
-      <c r="W2" t="s">
-        <v>164</v>
-      </c>
-      <c r="X2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AD2"/>
@@ -13535,6 +13659,193 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" t="s">
+        <v>312</v>
+      </c>
+      <c r="N1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" t="s">
+        <v>313</v>
+      </c>
+      <c r="P1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>314</v>
+      </c>
+      <c r="R1" t="s">
+        <v>315</v>
+      </c>
+      <c r="S1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" t="s">
+        <v>308</v>
+      </c>
+      <c r="U1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" t="s">
+        <v>61</v>
+      </c>
+      <c r="W1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>359</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" t="s">
+        <v>162</v>
+      </c>
+      <c r="K2" t="s">
+        <v>317</v>
+      </c>
+      <c r="L2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="O2" t="s">
+        <v>229</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>321</v>
+      </c>
+      <c r="R2" t="s">
+        <v>111</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="V2" t="s">
+        <v>91</v>
+      </c>
+      <c r="W2" t="s">
+        <v>164</v>
+      </c>
+      <c r="X2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <dimension ref="A1:AD2"/>
   <sheetViews>
@@ -13764,7 +14075,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
@@ -14021,7 +14332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
   <dimension ref="A1:V2"/>
   <sheetViews>
@@ -14185,7 +14496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
@@ -14334,7 +14645,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
   <dimension ref="A1:AH2"/>
   <sheetViews>
@@ -14581,7 +14892,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
@@ -14758,7 +15069,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
@@ -14979,7 +15290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
@@ -15200,7 +15511,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
@@ -15417,169 +15728,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
-  <dimension ref="A1:W2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
-        <v>354</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="Test@147" xr:uid="{00000000-0004-0000-3600-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -15922,6 +16070,169 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
+  <dimension ref="A1:W2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="Test@147" xr:uid="{00000000-0004-0000-3600-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656154C9-F525-4E04-BBB0-A63D4463202D}">
   <dimension ref="A1:AO2"/>
   <sheetViews>
@@ -16236,7 +16547,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17D8CD14-F2B6-41FF-B860-BBB543ECE21E}">
   <dimension ref="A1:AP2"/>
   <sheetViews>
@@ -16553,7 +16864,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE3D6DD-6BE6-4EB6-B2A0-BD80FDA3D32F}">
   <dimension ref="A1:AO2"/>
   <sheetViews>
@@ -16861,7 +17172,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6518BCCF-A49D-470B-A017-45C992076BFA}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
@@ -17099,7 +17410,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B7CD056-C366-41D6-BA4E-5671FEB95BD6}">
   <dimension ref="A1:AC2"/>
   <sheetViews>

</xml_diff>